<commit_message>
14 tests & refactoring
</commit_message>
<xml_diff>
--- a/Documentation/Testing/Test case for Currency Trader News Alert App.xlsx
+++ b/Documentation/Testing/Test case for Currency Trader News Alert App.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AndroidCollegeProject\Documentation\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53277B63-5831-4902-B9FE-D8FA940DA215}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB945D75-627F-4A59-BDF8-68ECAAB3E234}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="107">
   <si>
     <t>Test No.</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>CT-0001</t>
-  </si>
-  <si>
-    <t>Dev Acceptance:  Clear Main Actvity Screen</t>
   </si>
   <si>
     <t>Minor</t>
@@ -171,14 +168,6 @@
   <si>
     <t>1)  At the top of the screen 'Clear Option Selected' is displayed. 
 2)  Main display is blank and clear of all market data.</t>
-  </si>
-  <si>
-    <t>1)  Main dsiplay contains a scrollable list of all market data currently in the database.</t>
-  </si>
-  <si>
-    <t>1)  'EUR' and  'GBP', the previously selected currencies still have their checkboxes ticked / selected.
-2)  Main dsiplay remains unchanged unless selections have been made in bottom toolbar option 'Select Market Impacts(s)'.
-3)  If selections have been made in previous step - main display updates with new currency data by market impact.</t>
   </si>
   <si>
     <t>CT-0004</t>
@@ -251,9 +240,6 @@
     <t>Verify that currently selected currencies and market impacts are written out to the console window.</t>
   </si>
   <si>
-    <t>Verify that market data has been sucesssfully downloaded, converted, stored in database and displayed to main screen.</t>
-  </si>
-  <si>
     <t xml:space="preserve">1) Start application.
 2) Select top toolbar - 1st menu option:  'Update XML Market Data' 
 3) Select bottom toolbar - 1st menu option:  'Clear'.                                             
@@ -286,22 +272,139 @@
     <t>CT-0008</t>
   </si>
   <si>
-    <t>1)  Set an alert on a merket event - follow steps in test CT-0007 (Dev Acceptance: Set alert on market event)
+    <t>1)  User alert selected for deletion has been removed from list of user alerts on user alert screen.</t>
+  </si>
+  <si>
+    <t>CT-0009</t>
+  </si>
+  <si>
+    <t>Dev Acceptance: Delete user alert on previously set  market event</t>
+  </si>
+  <si>
+    <t>Verify that a previously set  user alert on a market event has been deleted.</t>
+  </si>
+  <si>
+    <t>1) Personal alerts screen closes.
+1)  User alerts screen opens containing the newly input personal alert and any previously set alerts (if any).
+2)  If the newly added alert's date or time is in the past, alert notification will fire.</t>
+  </si>
+  <si>
+    <t>Dev Acceptance: Set a personal alert</t>
+  </si>
+  <si>
+    <t>Verify that the user can set a personal alert on a date and time of their choosing, with accompanying title and description.</t>
+  </si>
+  <si>
+    <t>CT-0010</t>
+  </si>
+  <si>
+    <t>Dev Acceptance: Alert activation</t>
+  </si>
+  <si>
+    <t>Verify that a set alert activates.</t>
+  </si>
+  <si>
+    <t>1) Follow steps in test CT-0009 - setting date to today's date and time to a minute in the future.
+2) Wait for 1 minute.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) In approximately 1 minute an alert will sound, a notification will display and a new screen with an alert activated warning will display.
+2) User can click the 'Back' button which will return them to the user alert screen.
+</t>
+  </si>
+  <si>
+    <t>CT-0011</t>
+  </si>
+  <si>
+    <t>Dev Acceptance: User set time offset</t>
+  </si>
+  <si>
+    <t>Verify that user can set a time offset, so that all market data alerts can be activated by a set amount of time, either before or after the original scheduled alert time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Start application.
+2) Select top toolbar - 3rd menu option:  'Preferences' - preferences screen is displayed.
+3) User enters a  number between -60 and + 60 (inclusive), e.g. 10 and then clicks the 'Set' button.
+</t>
+  </si>
+  <si>
+    <t>1) Main screen is displayed.
+2) 'Times offset by' at the top of the screen will indicate the number of minutes market events are currently offset by, in this case 10 minutes as entered previously.
+3) All scrollable, market events have been updated by +10 minutes.</t>
+  </si>
+  <si>
+    <t>CT-0012</t>
+  </si>
+  <si>
+    <t>Verify that user has input correct value when setting a time offset.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Start application.
+2) Select top toolbar - 3rd menu option:  'Preferences' - preferences screen is displayed.
+3) User leaves input blank and clicks the 'Set' button.
+</t>
+  </si>
+  <si>
+    <t>1) Error message is displayed: 'Input must not be blank'</t>
+  </si>
+  <si>
+    <t>CT-0013</t>
+  </si>
+  <si>
+    <t>Dev Acceptance: Validate correct input for user time offset input - not a valid number</t>
+  </si>
+  <si>
+    <t>Dev Acceptance: Validate correct input for user time offset input - blank entry</t>
+  </si>
+  <si>
+    <t>Verify that user has input a valid number value when setting a time offset.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Start application.
+2) Select top toolbar - 3rd menu option:  'Preferences' - preferences screen is displayed.
+3) User enters non digit characters and clicks the 'Set' button.
+</t>
+  </si>
+  <si>
+    <t>1) Error message is displayed: 'Must be a number'</t>
+  </si>
+  <si>
+    <t>CT-0014</t>
+  </si>
+  <si>
+    <t>Dev Acceptance: Validate correct input for user time offset input - valid number between -60 and +60 inclusive</t>
+  </si>
+  <si>
+    <t>Verify that user has input a valid number value between -60 and +60 inclusive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Start application.
+2) Select top toolbar - 3rd menu option:  'Preferences' - preferences screen is displayed.
+3) User enters 100 and clicks the 'Set' button.
+</t>
+  </si>
+  <si>
+    <t>1) Error message is displayed: 'Number must be between plus or minus 60 minutes (inclusive)'.</t>
+  </si>
+  <si>
+    <t>Dev Acceptance:  Clear Main Activity Screen</t>
+  </si>
+  <si>
+    <t>1)  Main display contains a scrollable list of all market data currently in the database.</t>
+  </si>
+  <si>
+    <t>1)  'EUR' and  'GBP', the previously selected currencies still have their checkboxes ticked / selected.
+2)  Main display remains unchanged unless selections have been made in bottom toolbar option 'Select Market Impacts(s)'.
+3)  If selections have been made in previous step - main display updates with new currency data by market impact.</t>
+  </si>
+  <si>
+    <t>Verify that market data has been successfully downloaded, converted, stored in database and displayed to main screen.</t>
+  </si>
+  <si>
+    <t>1)  Set an alert on a market event - follow steps in test CT-0007 (Dev Acceptance: Set alert on market event)
 2)  On the User Alerts screen, select / click on the event to be deleted.
 3)  Dialog box opens: 'Delete this user alert ?'
 4)  Select 'OK'.</t>
-  </si>
-  <si>
-    <t>1)  User alert selected for deletion has been removed from list of user alerts on user alert screen.</t>
-  </si>
-  <si>
-    <t>CT-0009</t>
-  </si>
-  <si>
-    <t>Dev Acceptance: Delete user alert on previously set  market event</t>
-  </si>
-  <si>
-    <t>Verify that a previously set  user alert on a market event has been deleted.</t>
   </si>
   <si>
     <t>1) Select top toolbar - 1st menu option:  'User Alerts' - user alerts screen is displayed. 
@@ -309,38 +412,9 @@
 3) Personal alert screen is displayed
 4)  Enter title of alert.
 5) Enter description of alert.
-6)  Click 'Set Date' button and select a date using the datepicker displayed.
-7)  Click 'Set Time' button and select a time using the timepicker displayed.
+6)  Click 'Set Date' button and select a date using the date picker displayed.
+7)  Click 'Set Time' button and select a time using the time picker displayed.
 8) Click 'Set Alert' button.</t>
-  </si>
-  <si>
-    <t>1) Personal alerts screen closes.
-1)  User alerts screen opens containing the newly input personal alert and any previously set alerts (if any).
-2)  If the newly added alert's date or time is in the past, alert notification will fire.</t>
-  </si>
-  <si>
-    <t>Dev Acceptance: Set a personal alert</t>
-  </si>
-  <si>
-    <t>Verify that the user can set a personal alert on a date and time of their choosing, with accompanying title and description.</t>
-  </si>
-  <si>
-    <t>CT-0010</t>
-  </si>
-  <si>
-    <t>Dev Acceptance: Alert activation</t>
-  </si>
-  <si>
-    <t>Verify that a set alert activates.</t>
-  </si>
-  <si>
-    <t>1) Follow steps in test CT-0009 - setting date to today's date and time to a minute in the future.
-2) Wait for 1 minute.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) In approximately 1 minute an alert will sound, a notification will display and a new screen with an alert activated warning will display.
-2) User can click the 'Back' button which will return them to the user alert screen.
-</t>
   </si>
 </sst>
 </file>
@@ -757,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,23 +882,23 @@
         <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="2">
         <v>1.1000000000000001</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>4</v>
@@ -832,19 +906,19 @@
     </row>
     <row r="4" spans="1:9" ht="163.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="F4" s="2">
         <v>1.1000000000000001</v>
@@ -859,19 +933,19 @@
     </row>
     <row r="5" spans="1:9" ht="163.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F5" s="2">
         <v>1.1000000000000001</v>
@@ -886,19 +960,19 @@
     </row>
     <row r="6" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="F6" s="2">
         <v>1.1000000000000001</v>
@@ -913,19 +987,19 @@
     </row>
     <row r="7" spans="1:9" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="F7" s="2">
         <v>1.1000000000000001</v>
@@ -940,19 +1014,19 @@
     </row>
     <row r="11" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F11" s="2">
         <v>1.1000000000000001</v>
@@ -967,19 +1041,19 @@
     </row>
     <row r="13" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="F13" s="2">
         <v>1.1000000000000001</v>
@@ -994,19 +1068,19 @@
     </row>
     <row r="14" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F14" s="2">
         <v>1.1000000000000001</v>
@@ -1021,19 +1095,19 @@
     </row>
     <row r="15" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F15" s="2">
         <v>1.1000000000000001</v>
@@ -1048,19 +1122,19 @@
     </row>
     <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F16" s="2">
         <v>1.1000000000000001</v>
@@ -1070,6 +1144,115 @@
         <v>29</v>
       </c>
       <c r="I16" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>